<commit_message>
fetch employee status for mystatus page
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="151">
   <si>
     <t>Client</t>
   </si>
@@ -448,6 +448,27 @@
   </si>
   <si>
     <t>TitleIQQualityControl (only Search)</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Completed/Submitted</t>
+  </si>
+  <si>
+    <t>Hold/Suspended</t>
+  </si>
+  <si>
+    <t>ContactManager</t>
+  </si>
+  <si>
+    <t>Raised a Tickect</t>
+  </si>
+  <si>
+    <t>Placed for Review</t>
+  </si>
+  <si>
+    <t>Flipped</t>
   </si>
 </sst>
 </file>
@@ -922,10 +943,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V27"/>
+  <dimension ref="A1:X27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="R25" sqref="R25"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="X11" sqref="X11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -934,7 +955,7 @@
     <col min="18" max="18" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="15.75" thickBot="1">
+    <row r="1" spans="1:24" ht="15.75" thickBot="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1001,8 +1022,11 @@
       <c r="V1" s="9" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:22" ht="15.75" thickBot="1">
+      <c r="X1" s="9" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" ht="15.75" thickBot="1">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1069,8 +1093,11 @@
       <c r="V2" s="6" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="3" spans="1:22">
+      <c r="X2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -1131,8 +1158,11 @@
         <v>54</v>
       </c>
       <c r="V3" s="1"/>
-    </row>
-    <row r="4" spans="1:22">
+      <c r="X3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
@@ -1183,8 +1213,11 @@
         <v>66</v>
       </c>
       <c r="V4" s="1"/>
-    </row>
-    <row r="5" spans="1:22">
+      <c r="X4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
@@ -1233,8 +1266,11 @@
         <v>76</v>
       </c>
       <c r="V5" s="1"/>
-    </row>
-    <row r="6" spans="1:22">
+      <c r="X5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -1281,8 +1317,11 @@
         <v>83</v>
       </c>
       <c r="V6" s="1"/>
-    </row>
-    <row r="7" spans="1:22">
+      <c r="X6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="4" t="s">
@@ -1321,8 +1360,11 @@
         <v>91</v>
       </c>
       <c r="V7" s="1"/>
-    </row>
-    <row r="8" spans="1:22">
+      <c r="X7" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="4" t="s">
@@ -1360,7 +1402,7 @@
       </c>
       <c r="V8" s="1"/>
     </row>
-    <row r="9" spans="1:22">
+    <row r="9" spans="1:24">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="4" t="s">
@@ -1396,7 +1438,7 @@
       </c>
       <c r="V9" s="1"/>
     </row>
-    <row r="10" spans="1:22">
+    <row r="10" spans="1:24">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1428,7 +1470,7 @@
       <c r="U10" s="1"/>
       <c r="V10" s="1"/>
     </row>
-    <row r="11" spans="1:22">
+    <row r="11" spans="1:24">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1460,7 +1502,7 @@
       <c r="U11" s="1"/>
       <c r="V11" s="1"/>
     </row>
-    <row r="12" spans="1:22">
+    <row r="12" spans="1:24">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1492,7 +1534,7 @@
       <c r="U12" s="1"/>
       <c r="V12" s="1"/>
     </row>
-    <row r="13" spans="1:22">
+    <row r="13" spans="1:24">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1524,7 +1566,7 @@
       <c r="U13" s="1"/>
       <c r="V13" s="1"/>
     </row>
-    <row r="14" spans="1:22">
+    <row r="14" spans="1:24">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1556,7 +1598,7 @@
       <c r="U14" s="1"/>
       <c r="V14" s="1"/>
     </row>
-    <row r="15" spans="1:22">
+    <row r="15" spans="1:24">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1582,7 +1624,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="16" spans="1:22">
+    <row r="16" spans="1:24">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>

</xml_diff>